<commit_message>
final con named states
</commit_message>
<xml_diff>
--- a/closure.xlsx
+++ b/closure.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAVIDCORZO\Desktop\3_2\compi\Proyecto Final\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76A1EAD-616E-44FB-B13F-146592CC1118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8D3E48-9ECF-4E1F-AC8A-E2E4D6636C03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="big graph" sheetId="3" r:id="rId3"/>
+    <sheet name="exp" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="67">
   <si>
     <t>States</t>
   </si>
@@ -146,6 +148,96 @@
   </si>
   <si>
     <t>(a|b)*abb</t>
+  </si>
+  <si>
+    <t>start=19</t>
+  </si>
+  <si>
+    <t>dfa states</t>
+  </si>
+  <si>
+    <t>nfa states</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>{0,2,3,4,5,6,14,19}</t>
+  </si>
+  <si>
+    <t>{1,7,15}</t>
+  </si>
+  <si>
+    <t>{}</t>
+  </si>
+  <si>
+    <t>{5}</t>
+  </si>
+  <si>
+    <t>{9,17}</t>
+  </si>
+  <si>
+    <t>{12,10,13}</t>
+  </si>
+  <si>
+    <t>{11}</t>
+  </si>
+  <si>
+    <t>{10,13}</t>
+  </si>
+  <si>
+    <t>start=20</t>
+  </si>
+  <si>
+    <t>{20}</t>
+  </si>
+  <si>
+    <t>{{4},{6},{14}}</t>
+  </si>
+  <si>
+    <t>{{1},{7},{15}}</t>
+  </si>
+  <si>
+    <t>{0}</t>
+  </si>
+  <si>
+    <t>e-closure</t>
+  </si>
+  <si>
+    <t>{0,5}</t>
+  </si>
+  <si>
+    <t>{1}</t>
+  </si>
+  <si>
+    <t>{1,5}</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>{3,9}</t>
+  </si>
+  <si>
+    <t>{0,1,2,4,7,8}</t>
+  </si>
+  <si>
+    <t>{3,6,7,1,2,3,8,9}</t>
+  </si>
+  <si>
+    <t>{5,10}</t>
+  </si>
+  <si>
+    <t>{5,6,7,8,1,2,4}</t>
+  </si>
+  <si>
+    <t>{5,6,7,8,1,2,4,10}</t>
+  </si>
+  <si>
+    <t>{12}</t>
+  </si>
+  <si>
+    <t>IF nfa.accept_state in nfa_states: dfa es accepting state</t>
   </si>
 </sst>
 </file>
@@ -829,7 +921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC1BD4DA-9207-47B1-A881-835CEBE27BCE}">
   <dimension ref="D3:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3:J3"/>
     </sheetView>
   </sheetViews>
@@ -992,4 +1084,421 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{649A486F-89E8-4911-9F5E-4E9A5E8CA134}">
+  <dimension ref="B2:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="str">
+        <f>"ec("&amp;B4&amp;")"</f>
+        <v>ec({20})</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" t="str">
+        <f>"ec("&amp;B5&amp;")"</f>
+        <v>ec({1,7,15})</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="str">
+        <f>F5</f>
+        <v>{9,17}</v>
+      </c>
+      <c r="C6" t="str">
+        <f>"ec("&amp;B6&amp;")"</f>
+        <v>ec({9,17})</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" t="str">
+        <f>"ec("&amp;B7&amp;")"</f>
+        <v>ec({11})</v>
+      </c>
+      <c r="D7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" t="str">
+        <f>"ec("&amp;B11&amp;")"</f>
+        <v>ec({20})</v>
+      </c>
+      <c r="D11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" t="str">
+        <f>"ec("&amp;B12&amp;")"</f>
+        <v>ec({{1},{7},{15}})</v>
+      </c>
+      <c r="D12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3961749-7875-4EF4-8382-16DEC23EF66E}">
+  <dimension ref="B2:H15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="str">
+        <f>"ec("&amp;B3&amp;")"</f>
+        <v>ec({0})</v>
+      </c>
+      <c r="D3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="str">
+        <f>"ec("&amp;B4&amp;")"</f>
+        <v>ec({1})</v>
+      </c>
+      <c r="D4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="str">
+        <f>B2</f>
+        <v>dfa states</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" ref="C7:E7" si="0">C2</f>
+        <v>e-closure</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>nfa states</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>a</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" t="str">
+        <f>"ec("&amp;B8&amp;")"</f>
+        <v>ec({0})</v>
+      </c>
+      <c r="D8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" t="str">
+        <f>"ec("&amp;B9&amp;")"</f>
+        <v>ec({3,9})</v>
+      </c>
+      <c r="D9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" t="str">
+        <f>"ec("&amp;B10&amp;")"</f>
+        <v>ec({5})</v>
+      </c>
+      <c r="D10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" t="str">
+        <f>"ec("&amp;B11&amp;")"</f>
+        <v>ec({5,10})</v>
+      </c>
+      <c r="D11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" t="str">
+        <f>"ec("&amp;B12&amp;")"</f>
+        <v>ec({11})</v>
+      </c>
+      <c r="D12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" t="str">
+        <f>"ec("&amp;B13&amp;")"</f>
+        <v>ec({12})</v>
+      </c>
+      <c r="D13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" t="s">
+        <v>43</v>
+      </c>
+      <c r="H13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
lexer and scanner works, just missing the error messages
</commit_message>
<xml_diff>
--- a/closure.xlsx
+++ b/closure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAVIDCORZO\Desktop\3_2\compi\Proyecto Final\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8D3E48-9ECF-4E1F-AC8A-E2E4D6636C03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94AA7CE7-1F4B-48F1-BBC5-AEE02DA72112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1200" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1268,8 +1268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3961749-7875-4EF4-8382-16DEC23EF66E}">
   <dimension ref="B2:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="151" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1354,7 +1354,7 @@
         <v>53</v>
       </c>
       <c r="C8" t="str">
-        <f>"ec("&amp;B8&amp;")"</f>
+        <f t="shared" ref="C8:C13" si="1">"ec("&amp;B8&amp;")"</f>
         <v>ec({0})</v>
       </c>
       <c r="D8" t="s">
@@ -1378,7 +1378,7 @@
         <v>59</v>
       </c>
       <c r="C9" t="str">
-        <f>"ec("&amp;B9&amp;")"</f>
+        <f t="shared" si="1"/>
         <v>ec({3,9})</v>
       </c>
       <c r="D9" t="s">
@@ -1402,7 +1402,7 @@
         <v>44</v>
       </c>
       <c r="C10" t="str">
-        <f>"ec("&amp;B10&amp;")"</f>
+        <f t="shared" si="1"/>
         <v>ec({5})</v>
       </c>
       <c r="D10" t="s">
@@ -1426,7 +1426,7 @@
         <v>62</v>
       </c>
       <c r="C11" t="str">
-        <f>"ec("&amp;B11&amp;")"</f>
+        <f t="shared" si="1"/>
         <v>ec({5,10})</v>
       </c>
       <c r="D11" t="s">
@@ -1450,7 +1450,7 @@
         <v>47</v>
       </c>
       <c r="C12" t="str">
-        <f>"ec("&amp;B12&amp;")"</f>
+        <f t="shared" si="1"/>
         <v>ec({11})</v>
       </c>
       <c r="D12" t="s">
@@ -1474,7 +1474,7 @@
         <v>65</v>
       </c>
       <c r="C13" t="str">
-        <f>"ec("&amp;B13&amp;")"</f>
+        <f t="shared" si="1"/>
         <v>ec({12})</v>
       </c>
       <c r="D13" t="s">

</xml_diff>